<commit_message>
Atualizando a planilha jogos.xlsx
</commit_message>
<xml_diff>
--- a/jogos.xlsx
+++ b/jogos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2281,6 +2281,28 @@
         </is>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Incompleto</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>PS3</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Concluído</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização no arquivo jogos.xlsx
</commit_message>
<xml_diff>
--- a/jogos.xlsx
+++ b/jogos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2303,6 +2303,28 @@
         </is>
       </c>
     </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>Completo</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>PS3</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Platinado</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adicionando o arquivo jogos.xlsx
</commit_message>
<xml_diff>
--- a/jogos.xlsx
+++ b/jogos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D86"/>
+  <dimension ref="A1:D87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2325,6 +2325,28 @@
         </is>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>666</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>Incompleto</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Platinado</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizando o arquivo jogos.xlsx com novas informações em 2025-01-04 04:04:50
</commit_message>
<xml_diff>
--- a/jogos.xlsx
+++ b/jogos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2215,6 +2215,28 @@
         </is>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Teste Jogo PC</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Completo</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Concluído</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualizando o arquivo jogos.xlsx com novas informações em 2025-01-04 19:56:46
</commit_message>
<xml_diff>
--- a/jogos.xlsx
+++ b/jogos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2193,6 +2193,28 @@
         </is>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>teste de jogo ps5</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>Completo</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>PS5</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Concluído</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>